<commit_message>
TP1 Grupal, agregamos 1 caso mas de fatiga
</commit_message>
<xml_diff>
--- a/TP-1-2015-2C-Alumnos/ResultadoPruebas.xlsx
+++ b/TP-1-2015-2C-Alumnos/ResultadoPruebas.xlsx
@@ -881,12 +881,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="J14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+SALIDA: VACIO
+QUEDA LA APLICACIÓN COLGADA EN EL PROMP</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="24">
   <si>
     <t>CASO 01</t>
   </si>
@@ -955,6 +980,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>CASO 12</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1044,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1074,11 +1102,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1087,13 +1135,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1397,28 +1448,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
       <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1813,10 +1867,42 @@
       <c r="K13" s="4"/>
       <c r="L13" s="5"/>
     </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:G1"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>